<commit_message>
Chữa bài tập VN
</commit_message>
<xml_diff>
--- a/lay_capcha/registered_accounts.xlsx
+++ b/lay_capcha/registered_accounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>84383321820</t>
-        </is>
+      <c r="A2" t="n">
+        <v>84383321820</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -488,10 +486,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>84396360872</t>
-        </is>
+      <c r="A3" t="n">
+        <v>84396360872</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -515,10 +511,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>84315041690</t>
-        </is>
+      <c r="A4" t="n">
+        <v>84315041690</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -542,10 +536,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>84305303818</t>
-        </is>
+      <c r="A5" t="n">
+        <v>84305303818</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -569,10 +561,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>84345927948</t>
-        </is>
+      <c r="A6" t="n">
+        <v>84345927948</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -596,10 +586,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>84378408033</t>
-        </is>
+      <c r="A7" t="n">
+        <v>84378408033</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -623,10 +611,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>84335987003</t>
-        </is>
+      <c r="A8" t="n">
+        <v>84335987003</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -650,10 +636,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>84344078216</t>
-        </is>
+      <c r="A9" t="n">
+        <v>84344078216</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -677,10 +661,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>84375389598</t>
-        </is>
+      <c r="A10" t="n">
+        <v>84375389598</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -704,10 +686,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>84328861910</t>
-        </is>
+      <c r="A11" t="n">
+        <v>84328861910</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -731,10 +711,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>84377861708</t>
-        </is>
+      <c r="A12" t="n">
+        <v>84377861708</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -758,10 +736,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>84385551213</t>
-        </is>
+      <c r="A13" t="n">
+        <v>84385551213</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -785,10 +761,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>84362423607</t>
-        </is>
+      <c r="A14" t="n">
+        <v>84362423607</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -812,10 +786,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>84354222309</t>
-        </is>
+      <c r="A15" t="n">
+        <v>84354222309</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -839,10 +811,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>84368046503</t>
-        </is>
+      <c r="A16" t="n">
+        <v>84368046503</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -862,6 +832,276 @@
       <c r="E16" t="inlineStr">
         <is>
           <t>1971-05-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>84377215915</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BUI KHOA TRUONG KINH</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>buikinh537</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>hzxkznO36_</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1954-04-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>84307965136</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TRAN THINH HA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>tranha728</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>dbohtxL72*</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1958-11-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>84398006045</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>PHAN NGUYEN TRI TAN</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>phantan552</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>buxhrvR32*</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1999-09-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>84303354145</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>VO THANH HAI DOAN</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>vodoan137</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>egxuvbY22*</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1985-09-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>84374198711</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TRAN BINH THINH KHIEU</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>trankhieu660</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>jpebzeA56$</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1979-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>84318857412</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>VU THANG TUNG NHAN</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>vunhan216</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>fkjyohJ73@</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1980-09-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>84307033964</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BUI CHUNG HUNG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>buihung546</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>agybobF56$</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1980-11-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>84331765380</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>VU SAI TRUNG</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>vutrung943</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>yjmmjuE02*</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1997-02-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>84317185002</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>DANG TAT DINH</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>dangdinh270</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>rxxfjqU77_</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1954-10-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>84316963466</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>VU VAN DUC THI</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>vuthi211</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>zhvgzmA87@</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1958-12-14</t>
         </is>
       </c>
     </row>

</xml_diff>